<commit_message>
Includes all of Yesterday's data, converted to EST (GMT+5) to equate with Telog.
This version can run daily to continually update hourly meteomatics data from API
</commit_message>
<xml_diff>
--- a/rain_sites.xlsx
+++ b/rain_sites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3150" windowHeight="2873"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3150" windowHeight="2880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +99,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,110 +390,111 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>42.392794586999997</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>-71.084942663999996</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>42.28145</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>-71.400009999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>42.263779999999997</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>-71.099760000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>42.46114</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>-71.268069999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>42.365110000000001</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>-71.928117</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>42.261470000000003</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>-70.972290000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>42.32967</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>-71.046610000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>42.508220000000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>-71.094399999999993</v>
       </c>
     </row>

</xml_diff>